<commit_message>
updating part 1 closing issue 8
</commit_message>
<xml_diff>
--- a/Pilot_Input_Crop_Calendar.xlsx
+++ b/Pilot_Input_Crop_Calendar.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="108">
   <si>
     <t>Mode</t>
   </si>
@@ -391,18 +391,6 @@
     <t>05/10</t>
   </si>
   <si>
-    <t>init1_start</t>
-  </si>
-  <si>
-    <t>init1_end</t>
-  </si>
-  <si>
-    <t>init2_start</t>
-  </si>
-  <si>
-    <t>init2_end</t>
-  </si>
-  <si>
     <t>kc</t>
   </si>
   <si>
@@ -436,13 +424,16 @@
     <t>05/05</t>
   </si>
   <si>
-    <t>31/12</t>
-  </si>
-  <si>
     <t>Crop name: Sample</t>
   </si>
   <si>
     <t>region_1</t>
+  </si>
+  <si>
+    <t>30/10</t>
+  </si>
+  <si>
+    <t>30/12</t>
   </si>
 </sst>
 </file>
@@ -1379,96 +1370,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="11.85546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
-    <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" customWidth="1"/>
-    <col min="10" max="11" width="9.140625" customWidth="1"/>
-    <col min="12" max="16384" width="8.85546875" style="3"/>
+    <col min="1" max="3" width="11.85546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="71" t="s">
-        <v>93</v>
+        <v>39</v>
       </c>
       <c r="C1" s="72" t="s">
-        <v>94</v>
-      </c>
-      <c r="D1" s="71" t="s">
-        <v>95</v>
-      </c>
-      <c r="E1" s="72" t="s">
-        <v>96</v>
-      </c>
-      <c r="F1" s="73" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="74" t="s">
+      <c r="E1" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="75" t="s">
+      <c r="F1" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="I1" s="76" t="s">
+      <c r="G1" s="76" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="77" t="s">
+      <c r="H1" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="K1" s="78" t="s">
+      <c r="I1" s="78" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B2" s="79" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="C2" s="80" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D2" s="79" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="E2" s="80" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F2" s="79" t="s">
-        <v>8</v>
+        <v>103</v>
       </c>
       <c r="G2" s="80" t="s">
         <v>106</v>
       </c>
       <c r="H2" s="79" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="80" t="s">
         <v>107</v>
       </c>
-      <c r="I2" s="80" t="s">
-        <v>50</v>
-      </c>
-      <c r="J2" s="79" t="s">
-        <v>49</v>
-      </c>
-      <c r="K2" s="80" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1556,7 +1531,7 @@
         <v>23</v>
       </c>
       <c r="B6" s="89" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C6" s="90"/>
       <c r="D6" s="90"/>
@@ -1699,19 +1674,19 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1815,7 +1790,7 @@
         <v>85</v>
       </c>
       <c r="S24" s="51" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
@@ -2125,7 +2100,7 @@
     </row>
     <row r="37" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="81" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="M37" s="59" t="s">
         <v>22</v>
@@ -2177,16 +2152,16 @@
         <v>2</v>
       </c>
       <c r="C39" s="80" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D39" s="79" t="s">
         <v>8</v>
       </c>
       <c r="E39" s="80" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F39" s="79" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G39" s="80" t="s">
         <v>50</v>
@@ -2198,10 +2173,10 @@
         <v>7</v>
       </c>
       <c r="M39" s="59" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="N39" s="59" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.2">

</xml_diff>